<commit_message>
cleanup SMA since it is often copied
</commit_message>
<xml_diff>
--- a/indicators/Sma/Sma.Calc.xlsx
+++ b/indicators/Sma/Sma.Calc.xlsx
@@ -1,25 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AA8BCF-F997-44AE-B44D-F2AB884FC392}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89CECBE-BBA3-4106-BAAA-D9AEB681450D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SMA" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -124,7 +116,7 @@
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="_(&quot;$&quot;* #,##0.000000_);_(&quot;$&quot;* \(#,##0.000000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0.000000_);_(&quot;$&quot;* \(#,##0.000000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -650,7 +642,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="1" fillId="32" borderId="0" xfId="43" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="32" borderId="0" xfId="43" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1261,10 +1253,10 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="3" customWidth="1"/>
-    <col min="3" max="6" width="10.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="9" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.7109375" style="8" customWidth="1"/>
+    <col min="8" max="9" width="11" style="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.140625" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1736,6 +1728,9 @@
       <c r="G20" s="1">
         <v>84399624</v>
       </c>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
@@ -1759,15 +1754,15 @@
       <c r="G21" s="1">
         <v>80317680</v>
       </c>
-      <c r="H21" s="8">
+      <c r="H21" s="9">
         <f>AVERAGE(F2:F21)</f>
         <v>214.52499999999995</v>
       </c>
-      <c r="I21" s="8">
+      <c r="I21" s="9">
         <f>testdata[[#This Row],[SMA]]+0.025*testdata[[#This Row],[SMA]]</f>
         <v>219.88812499999995</v>
       </c>
-      <c r="J21" s="8">
+      <c r="J21" s="9">
         <f>testdata[[#This Row],[SMA]]-0.025*testdata[[#This Row],[SMA]]</f>
         <v>209.16187499999995</v>
       </c>
@@ -6309,15 +6304,15 @@
       <c r="G151" s="1">
         <v>33555464</v>
       </c>
-      <c r="H151" s="8">
+      <c r="H151" s="9">
         <f t="shared" si="2"/>
         <v>234.935</v>
       </c>
-      <c r="I151" s="8">
+      <c r="I151" s="9">
         <f>testdata[[#This Row],[SMA]]+0.025*testdata[[#This Row],[SMA]]</f>
         <v>240.80837500000001</v>
       </c>
-      <c r="J151" s="8">
+      <c r="J151" s="9">
         <f>testdata[[#This Row],[SMA]]-0.025*testdata[[#This Row],[SMA]]</f>
         <v>229.06162499999999</v>
       </c>

</xml_diff>

<commit_message>
chore: update docs (#381)
+semver: minor
</commit_message>
<xml_diff>
--- a/indicators/Sma/Sma.Calc.xlsx
+++ b/indicators/Sma/Sma.Calc.xlsx
@@ -1,25 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AA8BCF-F997-44AE-B44D-F2AB884FC392}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89CECBE-BBA3-4106-BAAA-D9AEB681450D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SMA" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -124,7 +116,7 @@
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="_(&quot;$&quot;* #,##0.000000_);_(&quot;$&quot;* \(#,##0.000000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0.000000_);_(&quot;$&quot;* \(#,##0.000000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -650,7 +642,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="1" fillId="32" borderId="0" xfId="43" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="32" borderId="0" xfId="43" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1261,10 +1253,10 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="3" customWidth="1"/>
-    <col min="3" max="6" width="10.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="9" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.7109375" style="8" customWidth="1"/>
+    <col min="8" max="9" width="11" style="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.140625" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1736,6 +1728,9 @@
       <c r="G20" s="1">
         <v>84399624</v>
       </c>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
@@ -1759,15 +1754,15 @@
       <c r="G21" s="1">
         <v>80317680</v>
       </c>
-      <c r="H21" s="8">
+      <c r="H21" s="9">
         <f>AVERAGE(F2:F21)</f>
         <v>214.52499999999995</v>
       </c>
-      <c r="I21" s="8">
+      <c r="I21" s="9">
         <f>testdata[[#This Row],[SMA]]+0.025*testdata[[#This Row],[SMA]]</f>
         <v>219.88812499999995</v>
       </c>
-      <c r="J21" s="8">
+      <c r="J21" s="9">
         <f>testdata[[#This Row],[SMA]]-0.025*testdata[[#This Row],[SMA]]</f>
         <v>209.16187499999995</v>
       </c>
@@ -6309,15 +6304,15 @@
       <c r="G151" s="1">
         <v>33555464</v>
       </c>
-      <c r="H151" s="8">
+      <c r="H151" s="9">
         <f t="shared" si="2"/>
         <v>234.935</v>
       </c>
-      <c r="I151" s="8">
+      <c r="I151" s="9">
         <f>testdata[[#This Row],[SMA]]+0.025*testdata[[#This Row],[SMA]]</f>
         <v>240.80837500000001</v>
       </c>
-      <c r="J151" s="8">
+      <c r="J151" s="9">
         <f>testdata[[#This Row],[SMA]]-0.025*testdata[[#This Row],[SMA]]</f>
         <v>229.06162499999999</v>
       </c>

</xml_diff>